<commit_message>
done all this proj for To 05 Nhom 02 Tri tue nhan tao
</commit_message>
<xml_diff>
--- a/data/DATACHATBOT.xlsx
+++ b/data/DATACHATBOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAO DUC\Desktop\BTL - Python\Chabot-AI--master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data of TuTran\A06- Kỳ 2 năm 3\Nhập môn AI\BTL TTNT\HealthCare-Chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9ED2F8-27E7-44C6-91E4-381A7D0762DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728BCBB7-EC2D-4F5D-BC00-48EA73C93E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{4BBA4252-B42F-4720-987D-A213D58092AE}"/>
+    <workbookView xWindow="28680" yWindow="2535" windowWidth="24240" windowHeight="13140" xr2:uid="{4BBA4252-B42F-4720-987D-A213D58092AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -1794,7 +1794,7 @@
     <t>mệt mỏi nên làm gì</t>
   </si>
   <si>
-    <t>tôi được tạo bởi các thành viên trong nhóm 10 môn lập trình python</t>
+    <t>tôi được tạo bởi các thành viên trong tổ 05 nhóm 02 Nhập môn trí tuệ nhân tạo</t>
   </si>
 </sst>
 </file>
@@ -1805,7 +1805,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2191,14 +2191,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEF706C-1EF7-4714-ADB9-2F8183B8584E}">
   <dimension ref="A1:B561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
-    <col min="2" max="2" width="194.5703125" customWidth="1"/>
+    <col min="1" max="1" width="75.09765625" customWidth="1"/>
+    <col min="2" max="2" width="194.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A309" s="2" t="s">
         <v>304</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A310" s="5" t="s">
         <v>306</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A311" s="3" t="s">
         <v>308</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="312" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A312" s="3" t="s">
         <v>310</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A313" s="3" t="s">
         <v>312</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A314" s="3" t="s">
         <v>314</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A315" s="3" t="s">
         <v>315</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A316" s="3" t="s">
         <v>561</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A317" s="3" t="s">
         <v>562</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A318" s="3" t="s">
         <v>304</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A319" s="3" t="s">
         <v>563</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A320" s="3" t="s">
         <v>564</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A321" s="3" t="s">
         <v>565</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A322" s="3" t="s">
         <v>566</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A323" s="3" t="s">
         <v>567</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A324" s="3" t="s">
         <v>568</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="325" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A325" s="3" t="s">
         <v>318</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A326" s="3" t="s">
         <v>320</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A327" s="3" t="s">
         <v>322</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A328" s="3" t="s">
         <v>324</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A329" s="3" t="s">
         <v>325</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A330" s="3" t="s">
         <v>322</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A331" s="3" t="s">
         <v>327</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A332" s="3" t="s">
         <v>320</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A333" s="3" t="s">
         <v>318</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A334" s="3" t="s">
         <v>329</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A335" s="3" t="s">
         <v>330</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="336" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A336" s="3" t="s">
         <v>331</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A337" s="3" t="s">
         <v>327</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="338" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A338" s="3" t="s">
         <v>332</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A339" s="3" t="s">
         <v>569</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A340" s="3" t="s">
         <v>333</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A341" s="3" t="s">
         <v>334</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A342" s="3" t="s">
         <v>335</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A343" s="3" t="s">
         <v>336</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A344" s="3" t="s">
         <v>338</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A345" s="3" t="s">
         <v>570</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A346" s="3" t="s">
         <v>339</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A347" s="3" t="s">
         <v>340</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A348" s="3" t="s">
         <v>341</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A349" s="3" t="s">
         <v>342</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A350" s="3" t="s">
         <v>344</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A351" s="3" t="s">
         <v>345</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A352" s="3" t="s">
         <v>571</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A353" s="3" t="s">
         <v>346</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A354" s="3" t="s">
         <v>347</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="355" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A355" s="3" t="s">
         <v>348</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A356" s="3" t="s">
         <v>350</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A357" s="3" t="s">
         <v>351</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A358" s="3" t="s">
         <v>352</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A359" s="3" t="s">
         <v>353</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A360" s="3" t="s">
         <v>354</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A361" s="3" t="s">
         <v>355</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="362" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A362" s="3" t="s">
         <v>572</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="363" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A363" s="3" t="s">
         <v>357</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A364" s="3" t="s">
         <v>358</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A365" s="3" t="s">
         <v>359</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A366" s="3" t="s">
         <v>360</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A367" s="3" t="s">
         <v>361</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="368" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A368" s="3" t="s">
         <v>362</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="369" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A369" s="3" t="s">
         <v>364</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="370" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A370" s="3" t="s">
         <v>365</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A371" s="3" t="s">
         <v>366</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A372" s="3" t="s">
         <v>367</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A373" s="3" t="s">
         <v>368</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A374" s="3" t="s">
         <v>369</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A375" s="3" t="s">
         <v>371</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A376" s="3" t="s">
         <v>372</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A377" s="3" t="s">
         <v>373</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="378" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A378" s="3" t="s">
         <v>374</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="379" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A379" s="3" t="s">
         <v>376</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="380" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A380" s="3" t="s">
         <v>377</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A381" s="3" t="s">
         <v>378</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="382" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A382" s="4" t="s">
         <v>379</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A383" s="3" t="s">
         <v>381</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="384" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A384" s="3" t="s">
         <v>382</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="385" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A385" s="3" t="s">
         <v>383</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="386" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A386" s="3" t="s">
         <v>384</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="387" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A387" s="4" t="s">
         <v>385</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A388" s="3" t="s">
         <v>387</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A389" s="3" t="s">
         <v>388</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="390" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A390" s="3" t="s">
         <v>389</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="391" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A391" s="4" t="s">
         <v>390</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="392" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A392" s="3" t="s">
         <v>392</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A393" s="3" t="s">
         <v>393</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="394" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A394" s="3" t="s">
         <v>394</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A395" s="3" t="s">
         <v>395</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A396" s="3" t="s">
         <v>396</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="397" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A397" s="3" t="s">
         <v>397</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="398" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A398" s="4" t="s">
         <v>398</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A399" s="3" t="s">
         <v>400</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="400" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A400" s="3" t="s">
         <v>401</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A401" s="3" t="s">
         <v>402</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="402" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A402" s="3" t="s">
         <v>403</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="403" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A403" s="3" t="s">
         <v>404</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A404" s="3" t="s">
         <v>405</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A405" s="3" t="s">
         <v>406</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A406" s="3" t="s">
         <v>407</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A407" s="3" t="s">
         <v>409</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A408" s="3" t="s">
         <v>410</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A409" s="3" t="s">
         <v>411</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A410" s="3" t="s">
         <v>412</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="411" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A411" s="4" t="s">
         <v>413</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A412" s="3" t="s">
         <v>415</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A413" s="3" t="s">
         <v>416</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="414" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A414" s="3" t="s">
         <v>417</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="415" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A415" s="3" t="s">
         <v>418</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A416" s="3" t="s">
         <v>419</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="417" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A417" s="3" t="s">
         <v>420</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="418" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A418" s="3" t="s">
         <v>421</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A419" s="3" t="s">
         <v>422</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="420" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A420" s="4" t="s">
         <v>423</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A421" s="3" t="s">
         <v>425</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="422" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A422" s="3" t="s">
         <v>426</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="423" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A423" s="3" t="s">
         <v>427</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="424" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A424" s="3" t="s">
         <v>428</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="425" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A425" s="3" t="s">
         <v>429</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="426" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A426" s="3" t="s">
         <v>430</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="427" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A427" s="4" t="s">
         <v>431</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A428" s="3" t="s">
         <v>433</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="429" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A429" s="3" t="s">
         <v>434</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="430" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A430" s="3" t="s">
         <v>435</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A431" s="3" t="s">
         <v>436</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A432" s="3" t="s">
         <v>437</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="433" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A433" s="3" t="s">
         <v>438</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="434" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A434" s="3" t="s">
         <v>439</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="435" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A435" s="3" t="s">
         <v>440</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="436" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A436" s="4" t="s">
         <v>441</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A437" s="3" t="s">
         <v>443</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="438" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A438" s="3" t="s">
         <v>444</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A439" s="3" t="s">
         <v>445</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A440" s="3" t="s">
         <v>446</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="441" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A441" s="3" t="s">
         <v>446</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="442" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A442" s="3" t="s">
         <v>447</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="443" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A443" s="3" t="s">
         <v>448</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="444" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A444" s="4" t="s">
         <v>449</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="445" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A445" s="3" t="s">
         <v>451</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="446" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A446" s="3" t="s">
         <v>452</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="447" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A447" s="3" t="s">
         <v>453</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A448" s="3" t="s">
         <v>454</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="449" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A449" s="3" t="s">
         <v>455</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="450" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A450" s="4" t="s">
         <v>456</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="451" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A451" s="3" t="s">
         <v>458</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="452" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A452" s="3" t="s">
         <v>459</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="453" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A453" s="3" t="s">
         <v>460</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="454" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A454" s="3" t="s">
         <v>461</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="455" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A455" s="3" t="s">
         <v>462</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="456" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A456" s="3" t="s">
         <v>463</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="457" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A457" s="4" t="s">
         <v>464</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="458" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A458" s="3" t="s">
         <v>466</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="459" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A459" s="3" t="s">
         <v>467</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="460" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A460" s="3" t="s">
         <v>468</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="461" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A461" s="3" t="s">
         <v>469</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="462" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A462" s="3" t="s">
         <v>470</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="463" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A463" s="3" t="s">
         <v>471</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="464" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A464" s="3" t="s">
         <v>472</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="465" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A465" s="4" t="s">
         <v>473</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="466" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A466" s="3" t="s">
         <v>475</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="467" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A467" s="3" t="s">
         <v>476</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="468" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A468" s="3" t="s">
         <v>477</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="469" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A469" s="3" t="s">
         <v>478</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="470" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A470" s="3" t="s">
         <v>479</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A471" s="3" t="s">
         <v>480</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="472" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A472" s="3" t="s">
         <v>481</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="473" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A473" s="3" t="s">
         <v>482</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="474" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A474" s="3" t="s">
         <v>483</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="475" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A475" s="3" t="s">
         <v>484</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="476" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A476" s="3" t="s">
         <v>485</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="477" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A477" s="3" t="s">
         <v>486</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="478" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A478" s="3" t="s">
         <v>487</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="479" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A479" s="3" t="s">
         <v>488</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="480" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A480" s="4" t="s">
         <v>489</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="481" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A481" s="3" t="s">
         <v>491</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="482" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A482" s="3" t="s">
         <v>492</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="483" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A483" s="3" t="s">
         <v>493</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="484" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A484" s="3" t="s">
         <v>494</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="485" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A485" s="3" t="s">
         <v>495</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="486" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A486" s="3" t="s">
         <v>496</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="487" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A487" s="3" t="s">
         <v>497</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A488" s="3" t="s">
         <v>499</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="489" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A489" s="3" t="s">
         <v>500</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="490" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A490" s="3" t="s">
         <v>501</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="491" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A491" s="3" t="s">
         <v>502</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="492" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A492" s="3" t="s">
         <v>503</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="493" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A493" s="3" t="s">
         <v>504</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="494" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A494" s="4" t="s">
         <v>505</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="495" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:2" ht="19.2" x14ac:dyDescent="0.25">
       <c r="A495" s="6" t="s">
         <v>507</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="496" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A496" s="3" t="s">
         <v>508</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A497" s="3" t="s">
         <v>509</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="498" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A498" s="3" t="s">
         <v>510</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="499" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A499" s="3" t="s">
         <v>511</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="500" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A500" s="3" t="s">
         <v>512</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="501" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A501" s="3" t="s">
         <v>513</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="502" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A502" s="3" t="s">
         <v>514</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="503" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A503" s="4" t="s">
         <v>517</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="504" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A504" s="4" t="s">
         <v>516</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="505" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A505" s="3" t="s">
         <v>518</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="506" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A506" s="3" t="s">
         <v>519</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="507" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A507" s="3" t="s">
         <v>520</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="508" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A508" s="3" t="s">
         <v>521</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="509" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A509" s="3" t="s">
         <v>522</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="510" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A510" s="3" t="s">
         <v>523</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="511" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A511" s="3" t="s">
         <v>524</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="512" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A512" s="3" t="s">
         <v>525</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="513" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A513" s="4" t="s">
         <v>526</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="514" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A514" s="3" t="s">
         <v>528</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="515" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A515" s="3" t="s">
         <v>529</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="516" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A516" s="3" t="s">
         <v>530</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="517" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A517" s="3" t="s">
         <v>531</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="518" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A518" s="3" t="s">
         <v>532</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="519" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A519" s="3" t="s">
         <v>533</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="520" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A520" s="3" t="s">
         <v>534</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="521" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A521" s="3" t="s">
         <v>535</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="522" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A522" s="3" t="s">
         <v>536</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="523" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A523" s="3" t="s">
         <v>537</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="524" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A524" s="3" t="s">
         <v>538</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="525" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A525" s="3" t="s">
         <v>539</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="526" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A526" s="3" t="s">
         <v>531</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="527" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A527" s="3" t="s">
         <v>540</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="528" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A528" s="4" t="s">
         <v>542</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="529" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A529" s="3" t="s">
         <v>544</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="530" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A530" s="3" t="s">
         <v>545</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="531" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A531" s="3" t="s">
         <v>546</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="532" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A532" s="3" t="s">
         <v>545</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="533" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A533" s="3" t="s">
         <v>547</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="534" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A534" s="3" t="s">
         <v>548</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="535" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A535" s="3" t="s">
         <v>549</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="536" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A536" s="3" t="s">
         <v>550</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="537" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A537" s="3" t="s">
         <v>551</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="538" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A538" s="3" t="s">
         <v>552</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="539" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A539" s="3" t="s">
         <v>553</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="540" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A540" s="2" t="s">
         <v>554</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="541" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A541" s="3" t="s">
         <v>556</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="542" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A542" s="3" t="s">
         <v>541</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="543" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A543" s="3" t="s">
         <v>557</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="544" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A544" s="3" t="s">
         <v>558</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="545" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A545" s="3" t="s">
         <v>556</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="546" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A546" s="3" t="s">
         <v>559</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="547" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A547" s="3" t="s">
         <v>560</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="548" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A548" s="3" t="s">
         <v>573</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="549" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A549" s="3" t="s">
         <v>575</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="550" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A550" s="3" t="s">
         <v>576</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="551" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A551" s="3" t="s">
         <v>577</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="552" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A552" s="3" t="s">
         <v>578</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="553" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A553" s="3" t="s">
         <v>579</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="554" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A554" s="3" t="s">
         <v>580</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="555" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A555" s="3" t="s">
         <v>581</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="556" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A556" s="3" t="s">
         <v>583</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="557" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A557" s="3" t="s">
         <v>584</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="558" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A558" s="3" t="s">
         <v>585</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="559" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A559" s="3" t="s">
         <v>586</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="560" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A560" s="3" t="s">
         <v>587</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="561" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
       <c r="A561" s="3" t="s">
         <v>588</v>
       </c>

</xml_diff>